<commit_message>
version 11/07/2016 - Début analyse orientée objet
</commit_message>
<xml_diff>
--- a/abreviations.xlsx
+++ b/abreviations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="abreviations" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
   <si>
     <t>CERN</t>
   </si>
@@ -235,13 +235,81 @@
   </si>
   <si>
     <t>F</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">RABOANARY Julien Amédée, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Gestion de qualité</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(support de cours, 2012-2013)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>RAKOTOARIMANANA Andriambao Johnson</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, UML 2, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(support de cours 2013-2014-2015)</t>
+    </r>
+  </si>
+  <si>
+    <t>UML 2.0 Laurent AUDIBERT</t>
+  </si>
+  <si>
+    <t>AOO</t>
+  </si>
+  <si>
+    <t>Analyse Orientée Objet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -299,6 +367,27 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -321,7 +410,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -330,6 +419,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -611,10 +701,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -633,42 +723,42 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="5" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="5" t="s">
-        <v>10</v>
+        <v>73</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="5" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -777,26 +867,26 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>45</v>
+        <v>10</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -825,26 +915,26 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>55</v>
+        <v>48</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -855,10 +945,21 @@
         <v>67</v>
       </c>
     </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState ref="A2:A30">
+    <sortCondition ref="A1"/>
+  </sortState>
   <hyperlinks>
-    <hyperlink ref="B20" r:id="rId1" tooltip="Joint Photographic Experts Group" display="http://fr.wikipedia.org/wiki/Joint_Photographic_Experts_Group"/>
-    <hyperlink ref="B26" r:id="rId2" tooltip="Système de gestion de base de données" display="http://fr.wikipedia.org/wiki/Syst%C3%A8me_de_gestion_de_base_de_donn%C3%A9es"/>
+    <hyperlink ref="B21" r:id="rId1" tooltip="Joint Photographic Experts Group" display="http://fr.wikipedia.org/wiki/Joint_Photographic_Experts_Group"/>
+    <hyperlink ref="B27" r:id="rId2" tooltip="Système de gestion de base de données" display="http://fr.wikipedia.org/wiki/Syst%C3%A8me_de_gestion_de_base_de_donn%C3%A9es"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -867,10 +968,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -926,7 +1027,32 @@
         <v>69</v>
       </c>
     </row>
+    <row r="10" spans="1:2" ht="15.75">
+      <c r="A10" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.75">
+      <c r="A11" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
critères de choix d'un langage (inachevé)
</commit_message>
<xml_diff>
--- a/abreviations.xlsx
+++ b/abreviations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="abreviations" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
   <si>
     <t>CERN</t>
   </si>
@@ -303,6 +303,54 @@
   </si>
   <si>
     <t>Analyse Orientée Objet</t>
+  </si>
+  <si>
+    <t>GAB</t>
+  </si>
+  <si>
+    <t>Guichet automatique bancaire</t>
+  </si>
+  <si>
+    <r>
+      <t>RAKOTONDRAHAJA Chantal</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, AOO, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(support de cours 2013-2014)</t>
+    </r>
+  </si>
+  <si>
+    <t>CRC</t>
+  </si>
+  <si>
+    <t>Classe - Responsabilité - Collaboration</t>
+  </si>
+  <si>
+    <t>https://fr.wikipedia.org/wiki/Langage_de_programmation</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>http://www.commentcamarche.net/faq/3964-programmation-criteres-de-choix-d-un-langage-framework</t>
+  </si>
+  <si>
+    <t>H</t>
   </si>
 </sst>
 </file>
@@ -701,10 +749,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -951,6 +999,22 @@
       </c>
       <c r="B30" s="1" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -968,10 +1032,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -1027,6 +1091,22 @@
         <v>69</v>
       </c>
     </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" t="s">
+        <v>83</v>
+      </c>
+    </row>
     <row r="10" spans="1:2" ht="15.75">
       <c r="A10" s="8" t="s">
         <v>70</v>
@@ -1043,12 +1123,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>72</v>
+    <row r="12" spans="1:2" ht="15.75">
+      <c r="A12" s="8" t="s">
+        <v>77</v>
       </c>
       <c r="B12">
         <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
version 14/07/1016 (début presentation MySQL)
</commit_message>
<xml_diff>
--- a/abreviations.xlsx
+++ b/abreviations.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\projet_soutenance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\soutenance_2016\soutaka\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="abreviations" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
   <si>
     <t>CERN</t>
   </si>
@@ -358,12 +358,33 @@
   <si>
     <t>Simple Object Access Protocol</t>
   </si>
+  <si>
+    <t>https://fr.wikipedia.org/wiki/Drupal</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Créez des applications android par Frédéric Espiau </t>
+  </si>
+  <si>
+    <t>fr.wikipédia.org, pour l’historique du langage Java et Html</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>https://fr.wikipedia.org/wiki/JavaScript</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -442,6 +463,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -464,7 +491,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -475,6 +502,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -758,17 +786,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="5"/>
-    <col min="2" max="2" width="97.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.375" style="5"/>
+    <col min="2" max="2" width="97.125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -776,7 +804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="5" t="s">
         <v>14</v>
       </c>
@@ -784,7 +812,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="5" t="s">
         <v>73</v>
       </c>
@@ -792,7 +820,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="5" t="s">
         <v>16</v>
       </c>
@@ -800,7 +828,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" s="5" t="s">
         <v>58</v>
       </c>
@@ -808,7 +836,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
@@ -816,7 +844,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" s="5" t="s">
         <v>18</v>
       </c>
@@ -824,7 +852,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" s="5" t="s">
         <v>20</v>
       </c>
@@ -832,7 +860,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" s="5" t="s">
         <v>22</v>
       </c>
@@ -840,7 +868,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2">
       <c r="A10" s="5" t="s">
         <v>24</v>
       </c>
@@ -848,7 +876,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2">
       <c r="A11" s="5" t="s">
         <v>26</v>
       </c>
@@ -856,7 +884,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2">
       <c r="A12" s="5" t="s">
         <v>28</v>
       </c>
@@ -864,7 +892,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2">
       <c r="A13" s="5" t="s">
         <v>30</v>
       </c>
@@ -872,7 +900,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2">
       <c r="A14" s="5" t="s">
         <v>32</v>
       </c>
@@ -880,7 +908,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2">
       <c r="A15" s="5" t="s">
         <v>34</v>
       </c>
@@ -888,7 +916,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2">
       <c r="A16" s="5" t="s">
         <v>36</v>
       </c>
@@ -896,7 +924,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17" s="5" t="s">
         <v>38</v>
       </c>
@@ -904,7 +932,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18" s="5" t="s">
         <v>40</v>
       </c>
@@ -912,7 +940,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="A19" s="5" t="s">
         <v>42</v>
       </c>
@@ -920,7 +948,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2">
       <c r="A20" s="5" t="s">
         <v>10</v>
       </c>
@@ -928,7 +956,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2">
       <c r="A21" s="5" t="s">
         <v>44</v>
       </c>
@@ -936,7 +964,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2">
       <c r="A22" s="5" t="s">
         <v>46</v>
       </c>
@@ -944,7 +972,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2">
       <c r="A23" s="5" t="s">
         <v>50</v>
       </c>
@@ -952,7 +980,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2">
       <c r="A24" s="5" t="s">
         <v>51</v>
       </c>
@@ -960,7 +988,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2">
       <c r="A25" s="5" t="s">
         <v>53</v>
       </c>
@@ -968,7 +996,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2">
       <c r="A26" s="5" t="s">
         <v>48</v>
       </c>
@@ -976,7 +1004,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2">
       <c r="A27" s="5" t="s">
         <v>54</v>
       </c>
@@ -984,7 +1012,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2">
       <c r="A28" s="5" t="s">
         <v>56</v>
       </c>
@@ -992,7 +1020,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2">
       <c r="A29" s="5" t="s">
         <v>66</v>
       </c>
@@ -1000,7 +1028,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2">
       <c r="A30" s="5" t="s">
         <v>4</v>
       </c>
@@ -1008,7 +1036,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2">
       <c r="A31" s="5" t="s">
         <v>75</v>
       </c>
@@ -1016,7 +1044,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2">
       <c r="A32" s="5" t="s">
         <v>78</v>
       </c>
@@ -1024,7 +1052,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2">
       <c r="A33" s="5" t="s">
         <v>84</v>
       </c>
@@ -1047,18 +1075,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="104.5703125" customWidth="1"/>
+    <col min="1" max="1" width="104.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1066,7 +1094,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1074,7 +1102,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1082,7 +1110,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>62</v>
       </c>
@@ -1090,7 +1118,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>64</v>
       </c>
@@ -1098,7 +1126,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>68</v>
       </c>
@@ -1106,7 +1134,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>80</v>
       </c>
@@ -1114,7 +1142,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" s="9" t="s">
         <v>82</v>
       </c>
@@ -1122,36 +1150,68 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15">
+      <c r="A10" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15.75">
+      <c r="A13" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="B10">
+      <c r="B13">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+    <row r="14" spans="1:2" ht="15.75">
+      <c r="A14" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="B11">
+      <c r="B14">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+    <row r="15" spans="1:2" ht="15.75">
+      <c r="A15" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="B12">
+      <c r="B15">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
         <v>72</v>
       </c>
-      <c r="B13">
+      <c r="B16">
         <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15">
+      <c r="A17" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B17">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
version 15/07/2016 (Chapitre 6:outils de développement)
</commit_message>
<xml_diff>
--- a/abreviations.xlsx
+++ b/abreviations.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\soutenance_2016\soutaka\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\projet_soutenance\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="abreviations" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="123">
   <si>
     <t>CERN</t>
   </si>
@@ -379,12 +379,194 @@
   <si>
     <t>K</t>
   </si>
+  <si>
+    <t>https://fr.wikipedia.org/wiki/MySQL</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">RANAIVOHARINIRIANA Tanjona, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">JavaScript, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(support de cours, 2012-2013)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>RAKOTONDRAHAJA Clarel</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, SGBDR,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (support de cours 2014-2015)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">RASANDIMANANA Tanjona Tsioharana, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">MySQL, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(support de cours, 2010-2011)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">RANDRIANTSOA Lalaina Thierry, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">PHP, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(support de cours, 2012-2013)</t>
+    </r>
+  </si>
+  <si>
+    <t>XML</t>
+  </si>
+  <si>
+    <t>Extensible Markup Language</t>
+  </si>
+  <si>
+    <t>AJAX</t>
+  </si>
+  <si>
+    <t>Asynchronous JavaScript</t>
+  </si>
+  <si>
+    <t>XHTML</t>
+  </si>
+  <si>
+    <t>Extensible HyperText Markup Language</t>
+  </si>
+  <si>
+    <t>Standard Generalized Markup Language</t>
+  </si>
+  <si>
+    <t>SGML</t>
+  </si>
+  <si>
+    <t>CSS</t>
+  </si>
+  <si>
+    <t>Cascade Style Sheet</t>
+  </si>
+  <si>
+    <t>JS</t>
+  </si>
+  <si>
+    <t>JavaScript</t>
+  </si>
+  <si>
+    <t>HTTP</t>
+  </si>
+  <si>
+    <t>HyperText Transfer Protocol</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Uniform Resource Locator</t>
+  </si>
+  <si>
+    <t>ODBC</t>
+  </si>
+  <si>
+    <t>Open Database Connectivity</t>
+  </si>
+  <si>
+    <t>JDBC</t>
+  </si>
+  <si>
+    <t>Java DataBase Connectivity</t>
+  </si>
+  <si>
+    <t>RFC</t>
+  </si>
+  <si>
+    <t>Requests For Comments</t>
+  </si>
+  <si>
+    <t>Information Technology Infrastructure Library</t>
+  </si>
+  <si>
+    <t>ITIL</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -784,19 +966,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.375" style="5"/>
-    <col min="2" max="2" width="97.125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="5"/>
+    <col min="2" max="2" width="97.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -804,7 +986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>14</v>
       </c>
@@ -812,7 +994,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>73</v>
       </c>
@@ -820,7 +1002,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>16</v>
       </c>
@@ -828,7 +1010,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>58</v>
       </c>
@@ -836,7 +1018,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
@@ -844,7 +1026,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>18</v>
       </c>
@@ -852,7 +1034,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>20</v>
       </c>
@@ -860,7 +1042,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>22</v>
       </c>
@@ -868,7 +1050,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>24</v>
       </c>
@@ -876,7 +1058,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>26</v>
       </c>
@@ -884,7 +1066,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>28</v>
       </c>
@@ -892,7 +1074,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>30</v>
       </c>
@@ -900,7 +1082,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>32</v>
       </c>
@@ -908,156 +1090,252 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="5" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="5" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="5" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="5" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="5" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="5" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B22" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="5" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="5" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="5" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="5" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B26" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="5" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="5" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B28" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="5" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="5" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B30" s="7" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="5" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="5" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="5" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="5" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>85</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1065,8 +1343,8 @@
     <sortCondition ref="A1"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="B21" r:id="rId1" tooltip="Joint Photographic Experts Group" display="http://fr.wikipedia.org/wiki/Joint_Photographic_Experts_Group"/>
-    <hyperlink ref="B27" r:id="rId2" tooltip="Système de gestion de base de données" display="http://fr.wikipedia.org/wiki/Syst%C3%A8me_de_gestion_de_base_de_donn%C3%A9es"/>
+    <hyperlink ref="B22" r:id="rId1" tooltip="Joint Photographic Experts Group" display="http://fr.wikipedia.org/wiki/Joint_Photographic_Experts_Group"/>
+    <hyperlink ref="B28" r:id="rId2" tooltip="Système de gestion de base de données" display="http://fr.wikipedia.org/wiki/Syst%C3%A8me_de_gestion_de_base_de_donn%C3%A9es"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -1075,18 +1353,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="104.625" customWidth="1"/>
+    <col min="1" max="1" width="104.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1094,7 +1372,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1102,7 +1380,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1110,7 +1388,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>62</v>
       </c>
@@ -1118,7 +1396,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>64</v>
       </c>
@@ -1126,7 +1404,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>68</v>
       </c>
@@ -1134,7 +1412,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>80</v>
       </c>
@@ -1142,7 +1420,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>82</v>
       </c>
@@ -1150,7 +1428,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>86</v>
       </c>
@@ -1158,7 +1436,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>89</v>
       </c>
@@ -1166,7 +1444,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>91</v>
       </c>
@@ -1174,44 +1452,90 @@
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15.75">
-      <c r="A13" s="8" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>93</v>
+      </c>
+      <c r="B12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="9"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="9"/>
+    </row>
+    <row r="16" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="B13">
+      <c r="B16">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15.75">
-      <c r="A14" s="8" t="s">
+    <row r="17" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="B14">
+      <c r="B17">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15.75">
-      <c r="A15" s="8" t="s">
+    <row r="18" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="B15">
+      <c r="B18">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
+    <row r="19" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>72</v>
       </c>
-      <c r="B16">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="15">
-      <c r="A17" s="7" t="s">
+      <c r="B23">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="B17">
-        <v>5</v>
+      <c r="B24">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
version 18/07/2016 (Partie 3:resultat obtenu)->code source - capture d'ecran inachevé
</commit_message>
<xml_diff>
--- a/abreviations.xlsx
+++ b/abreviations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="abreviations" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="127">
   <si>
     <t>CERN</t>
   </si>
@@ -560,6 +560,18 @@
   </si>
   <si>
     <t>ITIL</t>
+  </si>
+  <si>
+    <t>https://fr.wikipedia.org/wiki/Sublime_Text</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>https://fr.wikipedia.org/wiki/ArgoUML</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -968,7 +980,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
@@ -1355,8 +1367,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1461,10 +1473,20 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
+      <c r="A13" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B13" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
+      <c r="A14" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="B14" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="16" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">

</xml_diff>

<commit_message>
Reste à faire (résumé)
</commit_message>
<xml_diff>
--- a/abreviations.xlsx
+++ b/abreviations.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\projet_soutenance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\soutenance_2016\soutaka\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -578,7 +578,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -980,33 +980,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B45" sqref="A1:B45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="5"/>
-    <col min="2" max="2" width="97.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.375" style="5"/>
+    <col min="2" max="2" width="97.125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
+      <c r="A1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" s="5" t="s">
-        <v>14</v>
+        <v>101</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="5" t="s">
         <v>73</v>
       </c>
@@ -1014,7 +1014,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="5" t="s">
         <v>16</v>
       </c>
@@ -1022,271 +1022,271 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:2">
+      <c r="A5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+    <row r="7" spans="1:2">
+      <c r="A7" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+    <row r="10" spans="1:2">
+      <c r="A10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+    <row r="11" spans="1:2">
+      <c r="A11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+    <row r="12" spans="1:2">
+      <c r="A12" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+    <row r="13" spans="1:2">
+      <c r="A13" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+    <row r="14" spans="1:2">
+      <c r="A14" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+    <row r="16" spans="1:2">
+      <c r="A16" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+    <row r="17" spans="1:2">
+      <c r="A17" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B17" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+    <row r="18" spans="1:2">
+      <c r="A18" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B19" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+    <row r="20" spans="1:2">
+      <c r="A20" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+    <row r="21" spans="1:2">
+      <c r="A21" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+    <row r="22" spans="1:2">
+      <c r="A22" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+    <row r="23" spans="1:2">
+      <c r="A23" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+    <row r="24" spans="1:2">
+      <c r="A24" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+    <row r="25" spans="1:2">
+      <c r="A25" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+    <row r="26" spans="1:2">
+      <c r="A26" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B28" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+    <row r="29" spans="1:2">
+      <c r="A29" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
+    <row r="32" spans="1:2">
+      <c r="A32" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+    <row r="33" spans="1:2">
+      <c r="A33" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
+    <row r="34" spans="1:2">
+      <c r="A34" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
+    <row r="35" spans="1:2">
+      <c r="A35" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
+    <row r="36" spans="1:2">
+      <c r="A36" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B37" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2">
       <c r="A38" s="5" t="s">
         <v>106</v>
       </c>
@@ -1294,69 +1294,69 @@
         <v>105</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2">
       <c r="A39" s="5" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
       <c r="A40" s="5" t="s">
-        <v>109</v>
+        <v>56</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
       <c r="A41" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2">
       <c r="A43" s="5" t="s">
-        <v>117</v>
+        <v>4</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
       <c r="A44" s="5" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
       <c r="A45" s="5" t="s">
-        <v>122</v>
+        <v>99</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:A30">
-    <sortCondition ref="A1"/>
+  <sortState ref="A2:A45">
+    <sortCondition ref="A2"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="B22" r:id="rId1" tooltip="Joint Photographic Experts Group" display="http://fr.wikipedia.org/wiki/Joint_Photographic_Experts_Group"/>
-    <hyperlink ref="B28" r:id="rId2" tooltip="Système de gestion de base de données" display="http://fr.wikipedia.org/wiki/Syst%C3%A8me_de_gestion_de_base_de_donn%C3%A9es"/>
+    <hyperlink ref="B28" r:id="rId1" tooltip="Joint Photographic Experts Group" display="http://fr.wikipedia.org/wiki/Joint_Photographic_Experts_Group"/>
+    <hyperlink ref="B37" r:id="rId2" tooltip="Système de gestion de base de données" display="http://fr.wikipedia.org/wiki/Syst%C3%A8me_de_gestion_de_base_de_donn%C3%A9es"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -1368,201 +1368,201 @@
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B14" sqref="A1:B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="104.5703125" customWidth="1"/>
+    <col min="2" max="2" width="104.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15">
+      <c r="A10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>94</v>
+      </c>
+      <c r="B12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>126</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15.75">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.75">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15.75">
+      <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15.75">
+      <c r="A19">
+        <v>6</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15.75">
+      <c r="A20">
+        <v>4</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15.75">
+      <c r="A21">
+        <v>5</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15.75">
+      <c r="A22">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="B22" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="15">
+      <c r="A24">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>80</v>
-      </c>
-      <c r="B7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="B8" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>86</v>
-      </c>
-      <c r="B9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="B10" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="B11" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>93</v>
-      </c>
-      <c r="B12" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="B13" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="B14" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="B17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="B18">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B19">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B20">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B21">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B22">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>72</v>
-      </c>
-      <c r="B23">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
+      <c r="B24" s="7" t="s">
         <v>88</v>
-      </c>
-      <c r="B24">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A8" r:id="rId1"/>
+    <hyperlink ref="B8" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>